<commit_message>
updated the excel path and read values from excel and fix issues of education tab,
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -8,24 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaik\Downloads\Mars_AdvancedTask\src\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C64CE2-E4CC-438F-AB48-F0693E2E5869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07647C88-6718-4EB4-9072-D3A2959CACD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
     <sheet name="SignIn" sheetId="1" r:id="rId2"/>
-    <sheet name="Profile" sheetId="2" r:id="rId3"/>
-    <sheet name="EditProfile" sheetId="6" r:id="rId4"/>
-    <sheet name="EnterShareSkill" sheetId="4" r:id="rId5"/>
-    <sheet name="EditShareSkill" sheetId="5" r:id="rId6"/>
+    <sheet name="Education" sheetId="7" r:id="rId3"/>
+    <sheet name="Language" sheetId="8" r:id="rId4"/>
+    <sheet name="Profile" sheetId="2" r:id="rId5"/>
+    <sheet name="EditProfile" sheetId="6" r:id="rId6"/>
+    <sheet name="EnterShareSkill" sheetId="4" r:id="rId7"/>
+    <sheet name="EditShareSkill" sheetId="5" r:id="rId8"/>
+    <sheet name="Certificate" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet4" sheetId="10" r:id="rId10"/>
+    <sheet name="Sheet5" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet6" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet7" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
   <si>
     <t>Url</t>
   </si>
@@ -202,6 +209,42 @@
   </si>
   <si>
     <t>Learning selenium</t>
+  </si>
+  <si>
+    <t>dropDownListuni</t>
+  </si>
+  <si>
+    <t>JNTUH</t>
+  </si>
+  <si>
+    <t>Bachelor Degree</t>
+  </si>
+  <si>
+    <t>bachelor</t>
+  </si>
+  <si>
+    <t>addLang</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>languageModify</t>
+  </si>
+  <si>
+    <t>Telugu</t>
+  </si>
+  <si>
+    <t>cert</t>
+  </si>
+  <si>
+    <t>certFrom</t>
+  </si>
+  <si>
+    <t>certificationmodify</t>
+  </si>
+  <si>
+    <t>QTP</t>
   </si>
 </sst>
 </file>
@@ -655,12 +698,60 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B7C2AF-91BD-4177-A762-DEC174C8EF6F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F7B793-B805-4E73-B133-A09795015067}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BDFE76B-4615-4B50-8B8A-7BBC1277828E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C31807-18F4-4928-B1A2-FC1C6386A9DB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,11 +795,80 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC01F813-1B3D-47B7-B3F6-3832F229BAAE}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DD5FDD1-4D2F-4990-90BE-A604E5D39D6D}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,7 +952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F29D27-E839-4753-B8F8-BE6B563FA11B}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -881,7 +1041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62BC598-6354-4FB3-96B2-F83D377EF408}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -976,11 +1136,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA8CD366-4483-428E-B8BE-1947BB78560B}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -1016,4 +1176,41 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F7568F-A301-4809-A10C-38266A033DE3}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>